<commit_message>
adicionados novos recursos para o aplicativo
</commit_message>
<xml_diff>
--- a/base_dados/BaseDados.xlsx
+++ b/base_dados/BaseDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Modelos\VendasGalinhas\base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D930F420-F7D0-4834-BEE8-915C8628287C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C74C0B5-6A05-4720-89BB-7AE7A812D97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{76A520BB-3DFC-446D-92CB-E5703E97BECE}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,9 +62,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Ubuntu"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,10 +92,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,170 +418,168 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7AC5E6-FD47-45A0-B058-A57920CAFADE}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>53</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>115</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>180</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>257</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>338</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>829</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>424</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>1160</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>517</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>1540</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>597</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>1950</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>683</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>2400</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>774</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>2840</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>856</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="4">
+        <v>820</v>
+      </c>
+      <c r="C12" s="4">
         <v>3340</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>938</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="4">
+        <v>860</v>
+      </c>
+      <c r="C13" s="4">
         <v>3870</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>